<commit_message>
new results for table3
</commit_message>
<xml_diff>
--- a/Table2-100loactions.xlsx
+++ b/Table2-100loactions.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA\OSU\Tornado_proposal\Git\Two_Stage_Robust_Tornado_Problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78F5F3E-989C-4EBC-A5E4-F720857BB8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8D8C35-6C85-4EAF-A9BF-51D1EEC30EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Latex" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Best Bound</t>
   </si>
@@ -99,6 +100,33 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Population Dislocation</t>
+  </si>
+  <si>
+    <t>CCG Run time (sec.)</t>
+  </si>
+  <si>
+    <t>Subproblem Run time (sec.)</t>
+  </si>
+  <si>
+    <t>Subproblem Callbacks Run Time (sec.)</t>
+  </si>
+  <si>
+    <t>Uncertainty Set Check Run Time (sec.)</t>
+  </si>
+  <si>
+    <t>Retrofitting cost/budget</t>
+  </si>
+  <si>
+    <t>Budget \$</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Recovery cost/budget</t>
   </si>
 </sst>
 </file>
@@ -259,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -355,6 +383,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -908,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView topLeftCell="A12" zoomScale="96" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1248,4 +1282,248 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1263AB0E-6378-4269-94F2-4659E41B6DBD}">
+  <dimension ref="B4:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B4" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B5" s="33">
+        <v>5</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="34">
+        <v>16318</v>
+      </c>
+      <c r="E5" s="34">
+        <v>126.59</v>
+      </c>
+      <c r="F5" s="34">
+        <v>2</v>
+      </c>
+      <c r="G5" s="34">
+        <v>126.45</v>
+      </c>
+      <c r="H5" s="34">
+        <v>3.49</v>
+      </c>
+      <c r="I5" s="34">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="J5" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B6" s="33"/>
+      <c r="C6" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="34">
+        <v>13408</v>
+      </c>
+      <c r="E6" s="34">
+        <v>306.77</v>
+      </c>
+      <c r="F6" s="34">
+        <v>3</v>
+      </c>
+      <c r="G6" s="34">
+        <v>306.41000000000003</v>
+      </c>
+      <c r="H6" s="34">
+        <v>11.23</v>
+      </c>
+      <c r="I6" s="34">
+        <v>5.74</v>
+      </c>
+      <c r="J6" s="34">
+        <v>0.6</v>
+      </c>
+      <c r="K6" s="34">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B7" s="33"/>
+      <c r="C7" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="34">
+        <v>13091</v>
+      </c>
+      <c r="E7" s="34">
+        <v>300.22000000000003</v>
+      </c>
+      <c r="F7" s="34">
+        <v>3</v>
+      </c>
+      <c r="G7" s="34">
+        <v>299.87</v>
+      </c>
+      <c r="H7" s="34">
+        <v>10.6</v>
+      </c>
+      <c r="I7" s="34">
+        <v>5</v>
+      </c>
+      <c r="J7" s="34">
+        <v>0.3</v>
+      </c>
+      <c r="K7" s="34">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B8" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="34">
+        <v>17293</v>
+      </c>
+      <c r="E8" s="34">
+        <v>567.88</v>
+      </c>
+      <c r="F8" s="34">
+        <v>2</v>
+      </c>
+      <c r="G8" s="34">
+        <v>567.66</v>
+      </c>
+      <c r="H8" s="34">
+        <v>3.1</v>
+      </c>
+      <c r="I8" s="34">
+        <v>0</v>
+      </c>
+      <c r="J8" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B9" s="33"/>
+      <c r="C9" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="34">
+        <v>14236</v>
+      </c>
+      <c r="E9" s="34">
+        <v>716.36</v>
+      </c>
+      <c r="F9" s="34">
+        <v>2</v>
+      </c>
+      <c r="G9" s="34">
+        <v>716.12</v>
+      </c>
+      <c r="H9" s="34">
+        <v>4.66</v>
+      </c>
+      <c r="I9" s="34">
+        <v>0</v>
+      </c>
+      <c r="J9" s="34">
+        <v>0.62</v>
+      </c>
+      <c r="K9" s="34">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B10" s="33"/>
+      <c r="C10" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="34">
+        <v>13839</v>
+      </c>
+      <c r="E10" s="34">
+        <v>985.83</v>
+      </c>
+      <c r="F10" s="34">
+        <v>3</v>
+      </c>
+      <c r="G10" s="34">
+        <v>985.27</v>
+      </c>
+      <c r="H10" s="34">
+        <v>5.23</v>
+      </c>
+      <c r="I10" s="34">
+        <v>0</v>
+      </c>
+      <c r="J10" s="34">
+        <v>0.35</v>
+      </c>
+      <c r="K10" s="34">
+        <v>0.62</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modify best bound and best objective in the tables
</commit_message>
<xml_diff>
--- a/Table2-100loactions.xlsx
+++ b/Table2-100loactions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AAA\OSU\Tornado_proposal\Git\Two_Stage_Robust_Tornado_Problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A93F598-7FCD-4CCC-8C77-E9C38CDB1D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F26EBA-FEF0-4D12-8CA0-3E2958A8A97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -944,7 +944,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -980,11 +980,11 @@
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>2</v>
@@ -1285,11 +1285,11 @@
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>2</v>

</xml_diff>